<commit_message>
up biểu đồ time online của tk follow ngot.store.dc
</commit_message>
<xml_diff>
--- a/04. Ke Hoach/03. Ke hoach ca nhan/Sang/191029_kehoachcanhan_Sang.xlsx
+++ b/04. Ke Hoach/03. Ke hoach ca nhan/Sang/191029_kehoachcanhan_Sang.xlsx
@@ -220,6 +220,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -234,9 +237,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,7 +521,7 @@
   <dimension ref="A1:T61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -550,51 +550,51 @@
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14" t="s">
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="15" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
       <c r="K6" s="10"/>
       <c r="L6" s="11"/>
       <c r="M6" s="12"/>
@@ -615,10 +615,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="7"/>
       <c r="L7" s="8"/>
       <c r="M7" s="9"/>
@@ -794,16 +794,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:T5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B6:F6"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:T5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>